<commit_message>
Removing extra comments section #63
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/referral_confirmation.xlsx
+++ b/config/itech-aurum/forms/app/referral_confirmation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-63\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C622573-FAA3-4920-8721-54D583CA883C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11CEA4C-C53A-4BD3-836B-C4BB022CF47A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15825" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
   <si>
     <t>type</t>
   </si>
@@ -293,7 +293,7 @@
     <t>Please explain why the patient was not traced.</t>
   </si>
   <si>
-    <t>comments_2</t>
+    <t>selected(${trace}, 'yes')</t>
   </si>
 </sst>
 </file>
@@ -303,7 +303,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -372,12 +372,6 @@
     <font>
       <i/>
       <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -459,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -522,7 +516,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -908,13 +901,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1463,7 +1456,7 @@
       <c r="G21" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="38" t="s">
+      <c r="H21" s="36" t="s">
         <v>86</v>
       </c>
       <c r="I21" s="36"/>
@@ -1472,17 +1465,21 @@
     </row>
     <row r="22" spans="1:26">
       <c r="A22" s="34" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="36"/>
+        <v>59</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
+      <c r="F22" s="36" t="s">
+        <v>43</v>
+      </c>
       <c r="G22" s="36"/>
       <c r="H22" s="36"/>
       <c r="I22" s="36"/>
@@ -1491,16 +1488,16 @@
     </row>
     <row r="23" spans="1:26">
       <c r="A23" s="34" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E23" s="36"/>
       <c r="F23" s="36" t="s">
@@ -1517,18 +1514,16 @@
         <v>16</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>87</v>
+        <v>62</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>63</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E24" s="36"/>
-      <c r="F24" s="36" t="s">
-        <v>43</v>
-      </c>
+      <c r="F24" s="36"/>
       <c r="G24" s="36"/>
       <c r="H24" s="36"/>
       <c r="I24" s="36"/>
@@ -1536,29 +1531,10 @@
       <c r="K24" s="36"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="A25" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-    </row>
-    <row r="26" spans="1:26">
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>